<commit_message>
Log updates 5th Mar
</commit_message>
<xml_diff>
--- a/UncertainSea - Project Log.xlsx
+++ b/UncertainSea - Project Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perkinsth\Documents\GitHub\UncertainSea\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3565CDE9-A36A-4D7B-B75A-3B9886CD47F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26F65AB1-1748-48BD-8C63-F1B77F78671D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4824" yWindow="3924" windowWidth="13836" windowHeight="7176" activeTab="1" xr2:uid="{3D6C3FD5-F79E-43C8-B7E4-A5BABC36DA25}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3D6C3FD5-F79E-43C8-B7E4-A5BABC36DA25}"/>
   </bookViews>
   <sheets>
     <sheet name="Team list" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="120">
-  <si>
-    <t xml:space="preserve">Janet Peifer </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="105">
   <si>
     <t>Elizabeth Bradshaw</t>
   </si>
@@ -45,45 +42,18 @@
     <t>Aidan Slingsby</t>
   </si>
   <si>
-    <t>Rachel Perks</t>
-  </si>
-  <si>
-    <t>Jenny Dickinson</t>
-  </si>
-  <si>
-    <t>Robert McEwan</t>
-  </si>
-  <si>
     <t xml:space="preserve">Clare Postlethwaite </t>
   </si>
   <si>
-    <t>Joseph Elmes</t>
-  </si>
-  <si>
     <t>Jennifer Richardson</t>
   </si>
   <si>
-    <t>Paul Rowe</t>
-  </si>
-  <si>
-    <t>Tilly Harvey-Godfrey</t>
-  </si>
-  <si>
-    <t>Caryn Le Roux</t>
-  </si>
-  <si>
     <t>Guy Heathcote</t>
   </si>
   <si>
     <t>Jonathan Mackay</t>
   </si>
   <si>
-    <t xml:space="preserve">Andrew Broderick </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clare Lewis </t>
-  </si>
-  <si>
     <t>tom.howard@metoffice.gov.uk</t>
   </si>
   <si>
@@ -150,20 +120,9 @@
     <t>Mef Office</t>
   </si>
   <si>
-    <t xml:space="preserve">UoLeeds </t>
-  </si>
-  <si>
     <t>Relative sizes of Unc at different timeframes</t>
   </si>
   <si>
-    <t>Info</t>
-  </si>
-  <si>
-    <t>Ex-WRN
-visualisation of distributions
-complex data</t>
-  </si>
-  <si>
     <t xml:space="preserve">could we consider more of the social impact e.g. which areas of society might be most impacted? </t>
   </si>
   <si>
@@ -173,9 +132,6 @@
     <t>BGS</t>
   </si>
   <si>
-    <t>Met Office</t>
-  </si>
-  <si>
     <t>Project Focus</t>
   </si>
   <si>
@@ -198,12 +154,6 @@
   </si>
   <si>
     <t xml:space="preserve">UKCP18 land projections </t>
-  </si>
-  <si>
-    <t>Hydrology, Decomposing Uncertainty, Visualisation</t>
-  </si>
-  <si>
-    <t>Analytics, Catastrophe Modelling</t>
   </si>
   <si>
     <t>Tom Perkins</t>
@@ -349,9 +299,6 @@
     <t>a.slingsby@city.ac.uk</t>
   </si>
   <si>
-    <t>jenny.dickinson@naturalresourceswales.gov.uk</t>
-  </si>
-  <si>
     <t>Advisory?</t>
   </si>
   <si>
@@ -359,25 +306,10 @@
   </si>
   <si>
     <t>guy.heathcote@os.uk</t>
-  </si>
-  <si>
-    <t>Andrew Matthews</t>
-  </si>
-  <si>
-    <t>antt@noc.ac.uk</t>
-  </si>
-  <si>
-    <t>ee17jfp@leeds.ac.uk</t>
-  </si>
-  <si>
-    <t>Natural Resources Wales</t>
   </si>
   <si>
     <t>London City Uni; ex WRN
 Visualisation</t>
-  </si>
-  <si>
-    <t>Ordinance Survey</t>
   </si>
   <si>
     <t>NOC</t>
@@ -401,6 +333,27 @@
   </si>
   <si>
     <t>Y?</t>
+  </si>
+  <si>
+    <t>Ordnance Survey</t>
+  </si>
+  <si>
+    <t>Technical, 3D game development</t>
+  </si>
+  <si>
+    <t>Visualisation of distributions</t>
+  </si>
+  <si>
+    <t>Analytics, catastrophe Modelling</t>
+  </si>
+  <si>
+    <t>Hydrology, decomposing uncertainty, visualisation</t>
+  </si>
+  <si>
+    <t>BODC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Newcastle University </t>
   </si>
 </sst>
 </file>
@@ -1245,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A0C061-0127-4E39-8A7E-A237CD3D3F76}">
-  <dimension ref="B1:K21"/>
+  <dimension ref="B1:K10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1267,337 +1220,235 @@
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B1" s="22" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C1" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>50</v>
-      </c>
       <c r="F1" s="22" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="J1" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>40</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="2:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>55</v>
+        <v>101</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="I3" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="16.8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="16.8" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="39.6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="33.6" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="1"/>
+        <v>92</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>100</v>
+      </c>
       <c r="F7" s="4" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="I7" t="s">
-        <v>118</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>41</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="K7" s="5"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="9" spans="2:11" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>87</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="4" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="J9" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="2:11" ht="16.8" x14ac:dyDescent="0.25">
       <c r="B10" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1"/>
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="D10" s="20" t="s">
-        <v>104</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="4" t="s">
-        <v>105</v>
+      <c r="F10" t="s">
+        <v>18</v>
       </c>
       <c r="J10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="2:11" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="2:11" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="2:11" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="2:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="2:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="2:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="2:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="2:6" ht="16.8" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" t="s">
-        <v>113</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>108</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1607,14 +1458,11 @@
     <hyperlink ref="F5" r:id="rId3" xr:uid="{596CCC5C-9784-4F17-BA17-DA3C8DAEBAE3}"/>
     <hyperlink ref="F8" r:id="rId4" xr:uid="{66C05E1B-B29B-4C66-BEBB-CD0EA3316865}"/>
     <hyperlink ref="F7" r:id="rId5" xr:uid="{68FF1A40-A0A4-48C8-A5B3-881AEA83B7A2}"/>
-    <hyperlink ref="F12" r:id="rId6" xr:uid="{3A933109-5052-4503-966B-B3D5317F8E9E}"/>
-    <hyperlink ref="F10" r:id="rId7" xr:uid="{A6A798C4-160F-467C-8716-C1E792BD1B1C}"/>
-    <hyperlink ref="F6" r:id="rId8" xr:uid="{51F85D8D-B90D-45FB-82BF-7079D5A3C7B2}"/>
-    <hyperlink ref="F21" r:id="rId9" xr:uid="{ADA86623-F19A-4F7D-AD65-07834DB60791}"/>
-    <hyperlink ref="F9" r:id="rId10" display="mailto:ee17jfp@leeds.ac.uk" xr:uid="{249EDBEC-F3D1-4C82-A4B6-2D24B9BF96E2}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{A6A798C4-160F-467C-8716-C1E792BD1B1C}"/>
+    <hyperlink ref="F6" r:id="rId7" xr:uid="{51F85D8D-B90D-45FB-82BF-7079D5A3C7B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -1622,7 +1470,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96997B0F-1B5E-426D-81B8-125FF74E6826}">
   <dimension ref="B1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1637,208 +1485,208 @@
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B1" s="14" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F2" s="11"/>
     </row>
     <row r="3" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B3" s="8" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="285" x14ac:dyDescent="0.35">
       <c r="B4" s="8" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="F6" s="11"/>
     </row>
     <row r="7" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>64</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>80</v>
       </c>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F8" s="11"/>
     </row>
     <row r="9" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>98</v>
-      </c>
       <c r="E9" s="13" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="F9" s="11"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="F10" s="11"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F11" s="11"/>
     </row>
     <row r="12" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="F12" s="11"/>
     </row>
     <row r="13" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="F13" s="11"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="9"/>
@@ -1874,35 +1722,35 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update UncertainSea - Project Log.xlsx
</commit_message>
<xml_diff>
--- a/UncertainSea - Project Log.xlsx
+++ b/UncertainSea - Project Log.xlsx
@@ -1,39 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Documents\GitHub\UncertainSea\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perkinsth\Documents\GitHub\UncertainSea\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CC71C22-5CD2-4DBC-B5FB-4BD7AF34F478}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team list" sheetId="1" r:id="rId1"/>
     <sheet name="Data &amp; sources" sheetId="2" r:id="rId2"/>
+    <sheet name="Visuals" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="114">
   <si>
     <t>Elizabeth Bradshaw</t>
   </si>
@@ -324,20 +318,89 @@
     <t>Willis Re</t>
   </si>
   <si>
-    <t>London City Uni</t>
-  </si>
-  <si>
     <t>Newcastle University / Met Office</t>
   </si>
   <si>
     <t>thomas.perkins@willistowerswatson.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Example visualisation </t>
+  </si>
+  <si>
+    <t>National Trust</t>
+  </si>
+  <si>
+    <t>https://nationaltrust.maps.arcgis.com/apps/webappviewer/index.html?id=0bc569747210413a8c8598535a6b36e1</t>
+  </si>
+  <si>
+    <t>An example of map with data layer toggling on a 5km hexagonal grid</t>
+  </si>
+  <si>
+    <t>City University, London</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UKCP18 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Environment Agency </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview of marine projections </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCOPAC presentation </t>
+  </si>
+  <si>
+    <t>Summary of total coastal water level components</t>
+  </si>
+  <si>
+    <t>Median projection (a) and width of 17-83% uncertainty of likely range of local sea level risk in metre (b) in 2100 under RCP 8.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kopp et al (2014) </t>
+  </si>
+  <si>
+    <t>https://agupubs.onlinelibrary.wiley.com/doi/full/10.1002/2014EF000239</t>
+  </si>
+  <si>
+    <t>Probabilistic 21st and 22nd century sea‐level projections at a global network of tide‐gauge sites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra info </t>
+  </si>
+  <si>
+    <r>
+      <t>A global set of local sea‐level (LSL) projections. Between the years 2000 and 2100, we project a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>very likely</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF1C1D1E"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (90% probability) GSL rise of 0.5–1.2 m under representative concentration pathway (RCP) 8.5, 0.4–0.9 m under RCP 4.5, and 0.3–0.8 m under RCP 2.6. Site‐to‐site differences in LSL projections are due to varying non‐climatic background uplift or subsidence, oceanographic effects, and spatially variable responses of the geoid and the lithosphere to shrinking land ice. The Antarctic ice sheet (AIS) constitutes a growing share of variance in GSL and LSL projections. In the global average and at many locations, it is the dominant source of variance in late 21st century projections, though at some sites oceanographic processes contribute the largest share throughout the century. LSL rise dramatically reshapes flood risk, greatly increasing the expected number of “1‐in‐10” and “1‐in‐100” year events.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -368,6 +431,19 @@
       <sz val="10"/>
       <color rgb="FF333333"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF1C1D1E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF1C1D1E"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -419,7 +495,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -458,6 +534,30 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -480,23 +580,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>225497</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>100250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>2191803</xdr:colOff>
-      <xdr:row>57</xdr:row>
-      <xdr:rowOff>94342</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>526680</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>39413</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B43E5B7C-3A5C-41F4-9B7B-1150988E74EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{019FB2FE-4AD7-4245-AFE8-04FCA0E2D9E7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -512,52 +612,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8048625" y="4752975"/>
-          <a:ext cx="6822858" cy="7264762"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>3724275</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>3368418</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>97424</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C1707AB5-5176-4CBD-8619-EBA6FC4E28ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11706225" y="4448175"/>
-          <a:ext cx="4362828" cy="3101609"/>
+          <a:off x="11016762" y="783809"/>
+          <a:ext cx="4538912" cy="3132839"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -569,22 +625,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>72390</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>345062</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1063</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1141095</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>139418</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19707</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>60397</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{12D4DD74-267C-4D1D-8F65-D10F0DBB5E95}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F34FB539-5F99-4C76-B300-A7328F7C6657}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -593,7 +649,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -607,8 +663,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="681990" y="7286625"/>
-          <a:ext cx="3935730" cy="2530193"/>
+          <a:off x="1163091" y="3878298"/>
+          <a:ext cx="3914279" cy="2408760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -640,25 +696,143 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>106055</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>15932</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>521013</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>492</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D88BEFA0-1390-4245-A445-42E8C0DBAB27}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="924084" y="699491"/>
+          <a:ext cx="4652687" cy="3010148"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>311309</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>96462</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>314664</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>18522</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{988E12EC-1A9C-41BA-B8AA-5C0680B620CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6261633" y="780021"/>
+          <a:ext cx="3632155" cy="5472782"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>110843</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>4487415</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>168053</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>334272</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>46049</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 4">
+        <xdr:cNvPr id="7" name="Rectangle 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B52C80A5-9298-4C39-917E-47CD378C27E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA7A0198-DF0F-46F9-AEE3-E6F9220E5D0E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -666,8 +840,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="942975" y="9959693"/>
-          <a:ext cx="7021065" cy="400110"/>
+          <a:off x="605119" y="6219265"/>
+          <a:ext cx="3964977" cy="718402"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -784,23 +958,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>99175</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>110155</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>496185</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>93345</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>586854</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>127301</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
+        <xdr:cNvPr id="8" name="Picture 7" descr="EFT2-37-FIG-0001-b">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{50B86148-7EE2-4F54-BC83-26D9F6A7DECF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85FEB85F-AD0D-4E14-80B2-EF53BB749840}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -809,7 +983,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -823,33 +997,20 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3714750" y="9658350"/>
-          <a:ext cx="4563360" cy="2969895"/>
+          <a:off x="15966704" y="9198126"/>
+          <a:ext cx="4727313" cy="2032299"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
           </a:ext>
         </a:extLst>
       </xdr:spPr>
@@ -858,38 +1019,122 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>100632</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>59614</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>3647619</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>56475</xdr:rowOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>19389</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>97715</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPr id="9" name="Picture 8" descr="EFT2-37-FIG-0003-c">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AF20825B-4DCB-4475-9909-0457596D2022}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="12353925" y="4438650"/>
-          <a:ext cx="3647619" cy="5400000"/>
+          <a:off x="15968161" y="5617732"/>
+          <a:ext cx="4755888" cy="3396055"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>110380</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>115868</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>500008</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>161588</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="EFT2-37-FIG-0005-c">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73CD14E8-6A81-405A-A58B-8361EC8D1C6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="15720174" y="799427"/>
+          <a:ext cx="4625452" cy="4752190"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1193,172 +1438,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:J10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="50.28515625" customWidth="1"/>
-    <col min="13" max="13" width="78.28515625" customWidth="1"/>
-    <col min="14" max="14" width="41.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="50.33203125" customWidth="1"/>
+    <col min="13" max="13" width="78.33203125" customWidth="1"/>
+    <col min="14" max="14" width="41.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B1" s="18" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C2" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E2" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H2" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I2" s="18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="3" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>92</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>96</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>92</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>84</v>
+        <v>29</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>89</v>
+        <v>33</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -1370,88 +1587,114 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D7" s="15" t="s">
+      <c r="C8" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E8" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="19" t="s">
+      <c r="F8" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="J7" s="2"/>
-    </row>
-    <row r="8" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="J8" s="2"/>
+    </row>
+    <row r="9" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D9" s="17" t="s">
         <v>35</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" t="s">
-        <v>93</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>80</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+    <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D11" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1"/>
-    <hyperlink ref="F4" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="F8" r:id="rId4"/>
-    <hyperlink ref="F7" r:id="rId5"/>
-    <hyperlink ref="F9" r:id="rId6"/>
-    <hyperlink ref="F6" r:id="rId7"/>
-    <hyperlink ref="F2" r:id="rId8"/>
+    <hyperlink ref="F4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F5" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F3" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
@@ -1459,276 +1702,421 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:F19"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="D7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.7109375" customWidth="1"/>
-    <col min="5" max="5" width="68.5703125" customWidth="1"/>
-    <col min="6" max="6" width="106.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65.6640625" customWidth="1"/>
+    <col min="5" max="5" width="68.5546875" customWidth="1"/>
+    <col min="6" max="6" width="106.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B1" s="11" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D2" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E2" s="12" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
+      <c r="F2" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="2:6" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="171" x14ac:dyDescent="0.25">
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>41</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="195" x14ac:dyDescent="0.35">
+      <c r="B5" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="6" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>58</v>
+        <v>37</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B9" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>75</v>
-      </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="2:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="2:6" ht="39.6" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E13" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="2:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B13" s="5" t="s">
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="2:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="8"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="5" t="s">
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C15" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
       <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="E15" s="6"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>99</v>
+      </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-    <hyperlink ref="E5" r:id="rId2" display="https://www.ons.gov.uk/"/>
-    <hyperlink ref="E8" r:id="rId3" location="/geodemographics/imde2019/default/BTTTFFT/10/-0.1500/51.5200/" tooltip="https://maps.cdrc.ac.uk/#/geodemographics/imde2019/default/btttfft/10/-0.1500/51.5200/" display="/geodemographics/imde2019/default/BTTTFFT/10/-0.1500/51.5200/"/>
-    <hyperlink ref="E4" r:id="rId4"/>
-    <hyperlink ref="E10" r:id="rId5" display="https://www.ntslf.org/data"/>
-    <hyperlink ref="E11" r:id="rId6"/>
-    <hyperlink ref="E12" r:id="rId7"/>
-    <hyperlink ref="E13" r:id="rId8"/>
-    <hyperlink ref="E9" r:id="rId9"/>
-    <hyperlink ref="E7" r:id="rId10"/>
-    <hyperlink ref="F3" r:id="rId11" tooltip="https://ukclimateprojections-ui.metoffice.gov.uk/products/ms4_anomalies_subset_01"/>
-    <hyperlink ref="E3" r:id="rId12"/>
+    <hyperlink ref="E3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E6" r:id="rId2" display="https://www.ons.gov.uk/" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="E9" r:id="rId3" location="/geodemographics/imde2019/default/BTTTFFT/10/-0.1500/51.5200/" tooltip="https://maps.cdrc.ac.uk/#/geodemographics/imde2019/default/btttfft/10/-0.1500/51.5200/" display="/geodemographics/imde2019/default/BTTTFFT/10/-0.1500/51.5200/" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="E11" r:id="rId5" display="https://www.ntslf.org/data" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="E12" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="E13" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="E14" r:id="rId8" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="E8" r:id="rId10" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="F4" r:id="rId11" tooltip="https://ukclimateprojections-ui.metoffice.gov.uk/products/ms4_anomalies_subset_01" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="E4" r:id="rId12" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="E16" r:id="rId13" xr:uid="{31325251-827A-49F9-9AF9-1A5E959B4A06}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{2A072C98-F3AE-40A1-A3A0-FC717B09443B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
-  <drawing r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D35B6A1-3237-4189-9A4A-0312B7761B53}">
+  <dimension ref="A2:AI3"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W31" sqref="W31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.109375" customWidth="1"/>
+    <col min="18" max="18" width="4.109375" customWidth="1"/>
+    <col min="27" max="27" width="4.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="S2" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AB2" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="26"/>
+      <c r="AI2" s="26"/>
+    </row>
+    <row r="3" spans="1:35" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="23" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+      <c r="Q3" s="23"/>
+      <c r="S3" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="T3" s="21"/>
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21"/>
+      <c r="X3" s="21"/>
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AB3" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC3" s="22"/>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22"/>
+      <c r="AF3" s="22"/>
+      <c r="AG3" s="22"/>
+      <c r="AH3" s="22"/>
+      <c r="AI3" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="S3:Z3"/>
+    <mergeCell ref="S2:Z2"/>
+    <mergeCell ref="AB2:AI2"/>
+    <mergeCell ref="AB3:AI3"/>
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="K2:Q2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B2:I2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>